<commit_message>
perfstats hcr7 lowmed SR corrected
</commit_message>
<xml_diff>
--- a/output/Tables.xlsx
+++ b/output/Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\use\GitHub\FLBEIA_mseIBpil\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F27538-DCB5-4ED7-AA14-0F5C11B58682}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BD9C62D-3C60-4A5B-BEC6-DB12156A5E1C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1264,6 +1264,36 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="distributed" textRotation="90"/>
     </xf>
@@ -1272,12 +1302,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="distributed" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1306,32 +1330,8 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1739,40 +1739,40 @@
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E3" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="57"/>
-      <c r="L3" s="43"/>
+      <c r="E3" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="48"/>
     </row>
     <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="F4" s="43"/>
-      <c r="G4" s="42" t="s">
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="48"/>
+      <c r="G4" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="43"/>
-      <c r="I4" s="42" t="s">
+      <c r="H4" s="48"/>
+      <c r="I4" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="43"/>
-      <c r="K4" s="42" t="s">
+      <c r="J4" s="48"/>
+      <c r="K4" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="L4" s="43"/>
+      <c r="L4" s="48"/>
     </row>
     <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E5" s="21" t="s">
@@ -1807,28 +1807,28 @@
       <c r="D6" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="53" t="s">
+      <c r="E6" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="54"/>
-      <c r="G6" s="53" t="s">
+      <c r="F6" s="45"/>
+      <c r="G6" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="54"/>
-      <c r="I6" s="53" t="s">
+      <c r="H6" s="45"/>
+      <c r="I6" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="J6" s="54"/>
-      <c r="K6" s="53" t="s">
+      <c r="J6" s="45"/>
+      <c r="K6" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="L6" s="54"/>
+      <c r="L6" s="45"/>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="44" t="s">
+      <c r="C7" s="52" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="12" t="s">
@@ -1860,8 +1860,8 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="51"/>
-      <c r="C8" s="45"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="53"/>
       <c r="D8" s="13" t="s">
         <v>8</v>
       </c>
@@ -1891,8 +1891,8 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="51"/>
-      <c r="C9" s="46"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="54"/>
       <c r="D9" s="14" t="s">
         <v>9</v>
       </c>
@@ -1922,8 +1922,8 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="51"/>
-      <c r="C10" s="44" t="s">
+      <c r="B10" s="59"/>
+      <c r="C10" s="52" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="12" t="s">
@@ -1955,8 +1955,8 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="51"/>
-      <c r="C11" s="45"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="53"/>
       <c r="D11" s="13" t="s">
         <v>8</v>
       </c>
@@ -1986,8 +1986,8 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="51"/>
-      <c r="C12" s="46"/>
+      <c r="B12" s="59"/>
+      <c r="C12" s="54"/>
       <c r="D12" s="14" t="s">
         <v>9</v>
       </c>
@@ -2017,8 +2017,8 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="51"/>
-      <c r="C13" s="44" t="s">
+      <c r="B13" s="59"/>
+      <c r="C13" s="52" t="s">
         <v>14</v>
       </c>
       <c r="D13" s="12" t="s">
@@ -2050,8 +2050,8 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="51"/>
-      <c r="C14" s="45"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="53"/>
       <c r="D14" s="13" t="s">
         <v>8</v>
       </c>
@@ -2081,8 +2081,8 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="51"/>
-      <c r="C15" s="46"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="54"/>
       <c r="D15" s="14" t="s">
         <v>9</v>
       </c>
@@ -2112,8 +2112,8 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="51"/>
-      <c r="C16" s="47" t="s">
+      <c r="B16" s="59"/>
+      <c r="C16" s="55" t="s">
         <v>15</v>
       </c>
       <c r="D16" s="12" t="s">
@@ -2145,8 +2145,8 @@
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="51"/>
-      <c r="C17" s="48"/>
+      <c r="B17" s="59"/>
+      <c r="C17" s="56"/>
       <c r="D17" s="13" t="s">
         <v>8</v>
       </c>
@@ -2176,8 +2176,8 @@
       </c>
     </row>
     <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="52"/>
-      <c r="C18" s="49"/>
+      <c r="B18" s="60"/>
+      <c r="C18" s="57"/>
       <c r="D18" s="14" t="s">
         <v>9</v>
       </c>
@@ -2207,7 +2207,7 @@
       </c>
     </row>
     <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="39" t="s">
+      <c r="B19" s="49" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="26" t="s">
@@ -2242,7 +2242,7 @@
       </c>
     </row>
     <row r="20" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="40"/>
+      <c r="B20" s="50"/>
       <c r="C20" s="27" t="s">
         <v>23</v>
       </c>
@@ -2276,7 +2276,7 @@
     </row>
     <row r="21" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
-      <c r="B21" s="40"/>
+      <c r="B21" s="50"/>
       <c r="C21" s="28" t="s">
         <v>26</v>
       </c>
@@ -2309,7 +2309,7 @@
       </c>
     </row>
     <row r="22" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="41"/>
+      <c r="B22" s="51"/>
       <c r="C22" s="27" t="s">
         <v>27</v>
       </c>
@@ -2343,7 +2343,7 @@
     </row>
     <row r="23" spans="1:12" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
-      <c r="B23" s="39" t="s">
+      <c r="B23" s="49" t="s">
         <v>19</v>
       </c>
       <c r="C23" s="26" t="s">
@@ -2379,7 +2379,7 @@
     </row>
     <row r="24" spans="1:12" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10"/>
-      <c r="B24" s="40"/>
+      <c r="B24" s="50"/>
       <c r="C24" s="27" t="s">
         <v>29</v>
       </c>
@@ -2412,7 +2412,7 @@
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B25" s="40"/>
+      <c r="B25" s="50"/>
       <c r="C25" s="26" t="s">
         <v>20</v>
       </c>
@@ -2446,7 +2446,7 @@
     </row>
     <row r="26" spans="1:12" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="10"/>
-      <c r="B26" s="41"/>
+      <c r="B26" s="51"/>
       <c r="C26" s="27" t="s">
         <v>21</v>
       </c>
@@ -2777,12 +2777,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="E3:L3"/>
-    <mergeCell ref="K4:L4"/>
     <mergeCell ref="B19:B22"/>
     <mergeCell ref="B23:B26"/>
     <mergeCell ref="E4:F4"/>
@@ -2795,6 +2789,12 @@
     <mergeCell ref="B7:B18"/>
     <mergeCell ref="I6:J6"/>
     <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="E3:L3"/>
+    <mergeCell ref="K4:L4"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="61" orientation="landscape" verticalDpi="0" r:id="rId1"/>
@@ -2828,40 +2828,40 @@
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
     </row>
     <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E3" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="57"/>
-      <c r="L3" s="43"/>
+      <c r="E3" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="48"/>
     </row>
     <row r="4" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="F4" s="43"/>
-      <c r="G4" s="42" t="s">
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="48"/>
+      <c r="G4" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="43"/>
-      <c r="I4" s="42" t="s">
+      <c r="H4" s="48"/>
+      <c r="I4" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="43"/>
-      <c r="K4" s="42" t="s">
+      <c r="J4" s="48"/>
+      <c r="K4" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="L4" s="43"/>
+      <c r="L4" s="48"/>
     </row>
     <row r="5" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E5" s="37" t="s">
@@ -2896,28 +2896,28 @@
       <c r="D6" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="53" t="s">
+      <c r="E6" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="54"/>
-      <c r="G6" s="53" t="s">
+      <c r="F6" s="45"/>
+      <c r="G6" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="54"/>
-      <c r="I6" s="53" t="s">
+      <c r="H6" s="45"/>
+      <c r="I6" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="J6" s="54"/>
-      <c r="K6" s="53" t="s">
+      <c r="J6" s="45"/>
+      <c r="K6" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="L6" s="54"/>
+      <c r="L6" s="45"/>
     </row>
     <row r="7" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="44" t="s">
+      <c r="C7" s="52" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="12" t="s">
@@ -2949,8 +2949,8 @@
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="51"/>
-      <c r="C8" s="45"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="53"/>
       <c r="D8" s="13" t="s">
         <v>8</v>
       </c>
@@ -2980,8 +2980,8 @@
       </c>
     </row>
     <row r="9" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="51"/>
-      <c r="C9" s="46"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="54"/>
       <c r="D9" s="14" t="s">
         <v>9</v>
       </c>
@@ -3011,8 +3011,8 @@
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="51"/>
-      <c r="C10" s="44" t="s">
+      <c r="B10" s="59"/>
+      <c r="C10" s="52" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="12" t="s">
@@ -3044,8 +3044,8 @@
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="51"/>
-      <c r="C11" s="45"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="53"/>
       <c r="D11" s="13" t="s">
         <v>8</v>
       </c>
@@ -3075,8 +3075,8 @@
       </c>
     </row>
     <row r="12" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="51"/>
-      <c r="C12" s="46"/>
+      <c r="B12" s="59"/>
+      <c r="C12" s="54"/>
       <c r="D12" s="14" t="s">
         <v>9</v>
       </c>
@@ -3106,8 +3106,8 @@
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="51"/>
-      <c r="C13" s="44" t="s">
+      <c r="B13" s="59"/>
+      <c r="C13" s="52" t="s">
         <v>14</v>
       </c>
       <c r="D13" s="12" t="s">
@@ -3139,8 +3139,8 @@
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="51"/>
-      <c r="C14" s="45"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="53"/>
       <c r="D14" s="13" t="s">
         <v>8</v>
       </c>
@@ -3170,8 +3170,8 @@
       </c>
     </row>
     <row r="15" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="51"/>
-      <c r="C15" s="46"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="54"/>
       <c r="D15" s="14" t="s">
         <v>9</v>
       </c>
@@ -3201,8 +3201,8 @@
       </c>
     </row>
     <row r="16" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="51"/>
-      <c r="C16" s="47" t="s">
+      <c r="B16" s="59"/>
+      <c r="C16" s="55" t="s">
         <v>15</v>
       </c>
       <c r="D16" s="12" t="s">
@@ -3234,8 +3234,8 @@
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="51"/>
-      <c r="C17" s="48"/>
+      <c r="B17" s="59"/>
+      <c r="C17" s="56"/>
       <c r="D17" s="13" t="s">
         <v>8</v>
       </c>
@@ -3265,8 +3265,8 @@
       </c>
     </row>
     <row r="18" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="52"/>
-      <c r="C18" s="49"/>
+      <c r="B18" s="60"/>
+      <c r="C18" s="57"/>
       <c r="D18" s="14" t="s">
         <v>9</v>
       </c>
@@ -3296,7 +3296,7 @@
       </c>
     </row>
     <row r="19" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="39" t="s">
+      <c r="B19" s="49" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="26" t="s">
@@ -3331,7 +3331,7 @@
       </c>
     </row>
     <row r="20" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="40"/>
+      <c r="B20" s="50"/>
       <c r="C20" s="27" t="s">
         <v>23</v>
       </c>
@@ -3364,7 +3364,7 @@
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="40"/>
+      <c r="B21" s="50"/>
       <c r="C21" s="28" t="s">
         <v>26</v>
       </c>
@@ -3397,7 +3397,7 @@
       </c>
     </row>
     <row r="22" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="41"/>
+      <c r="B22" s="51"/>
       <c r="C22" s="27" t="s">
         <v>27</v>
       </c>
@@ -3430,7 +3430,7 @@
       </c>
     </row>
     <row r="23" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="39" t="s">
+      <c r="B23" s="49" t="s">
         <v>19</v>
       </c>
       <c r="C23" s="26" t="s">
@@ -3465,7 +3465,7 @@
       </c>
     </row>
     <row r="24" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="40"/>
+      <c r="B24" s="50"/>
       <c r="C24" s="27" t="s">
         <v>29</v>
       </c>
@@ -3498,7 +3498,7 @@
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B25" s="40"/>
+      <c r="B25" s="50"/>
       <c r="C25" s="26" t="s">
         <v>20</v>
       </c>
@@ -3531,7 +3531,7 @@
       </c>
     </row>
     <row r="26" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="41"/>
+      <c r="B26" s="51"/>
       <c r="C26" s="27" t="s">
         <v>21</v>
       </c>
@@ -3568,17 +3568,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="B7:B18"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="C16:C18"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E3:L3"/>
     <mergeCell ref="C4:D4"/>
@@ -3586,6 +3575,17 @@
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="B7:B18"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="61" orientation="landscape" verticalDpi="0" r:id="rId1"/>
@@ -3619,40 +3619,40 @@
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
     </row>
     <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E3" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="57"/>
-      <c r="L3" s="43"/>
+      <c r="E3" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="48"/>
     </row>
     <row r="4" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="F4" s="43"/>
-      <c r="G4" s="42" t="s">
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="48"/>
+      <c r="G4" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="43"/>
-      <c r="I4" s="42" t="s">
+      <c r="H4" s="48"/>
+      <c r="I4" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="43"/>
-      <c r="K4" s="42" t="s">
+      <c r="J4" s="48"/>
+      <c r="K4" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="L4" s="43"/>
+      <c r="L4" s="48"/>
     </row>
     <row r="5" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E5" s="37" t="s">
@@ -3687,28 +3687,28 @@
       <c r="D6" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="53" t="s">
+      <c r="E6" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="54"/>
-      <c r="G6" s="53" t="s">
+      <c r="F6" s="45"/>
+      <c r="G6" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="54"/>
-      <c r="I6" s="53" t="s">
+      <c r="H6" s="45"/>
+      <c r="I6" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="J6" s="54"/>
-      <c r="K6" s="53" t="s">
+      <c r="J6" s="45"/>
+      <c r="K6" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="L6" s="54"/>
+      <c r="L6" s="45"/>
     </row>
     <row r="7" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="44" t="s">
+      <c r="C7" s="52" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="12" t="s">
@@ -3740,8 +3740,8 @@
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="51"/>
-      <c r="C8" s="45"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="53"/>
       <c r="D8" s="13" t="s">
         <v>8</v>
       </c>
@@ -3771,8 +3771,8 @@
       </c>
     </row>
     <row r="9" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="51"/>
-      <c r="C9" s="46"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="54"/>
       <c r="D9" s="14" t="s">
         <v>9</v>
       </c>
@@ -3802,8 +3802,8 @@
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="51"/>
-      <c r="C10" s="44" t="s">
+      <c r="B10" s="59"/>
+      <c r="C10" s="52" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="12" t="s">
@@ -3835,8 +3835,8 @@
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="51"/>
-      <c r="C11" s="45"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="53"/>
       <c r="D11" s="13" t="s">
         <v>8</v>
       </c>
@@ -3866,8 +3866,8 @@
       </c>
     </row>
     <row r="12" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="51"/>
-      <c r="C12" s="46"/>
+      <c r="B12" s="59"/>
+      <c r="C12" s="54"/>
       <c r="D12" s="14" t="s">
         <v>9</v>
       </c>
@@ -3897,8 +3897,8 @@
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="51"/>
-      <c r="C13" s="44" t="s">
+      <c r="B13" s="59"/>
+      <c r="C13" s="52" t="s">
         <v>14</v>
       </c>
       <c r="D13" s="12" t="s">
@@ -3930,8 +3930,8 @@
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="51"/>
-      <c r="C14" s="45"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="53"/>
       <c r="D14" s="13" t="s">
         <v>8</v>
       </c>
@@ -3961,8 +3961,8 @@
       </c>
     </row>
     <row r="15" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="51"/>
-      <c r="C15" s="46"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="54"/>
       <c r="D15" s="14" t="s">
         <v>9</v>
       </c>
@@ -3992,8 +3992,8 @@
       </c>
     </row>
     <row r="16" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="51"/>
-      <c r="C16" s="47" t="s">
+      <c r="B16" s="59"/>
+      <c r="C16" s="55" t="s">
         <v>15</v>
       </c>
       <c r="D16" s="12" t="s">
@@ -4025,8 +4025,8 @@
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="51"/>
-      <c r="C17" s="48"/>
+      <c r="B17" s="59"/>
+      <c r="C17" s="56"/>
       <c r="D17" s="13" t="s">
         <v>8</v>
       </c>
@@ -4056,8 +4056,8 @@
       </c>
     </row>
     <row r="18" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="52"/>
-      <c r="C18" s="49"/>
+      <c r="B18" s="60"/>
+      <c r="C18" s="57"/>
       <c r="D18" s="14" t="s">
         <v>9</v>
       </c>
@@ -4087,7 +4087,7 @@
       </c>
     </row>
     <row r="19" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="39" t="s">
+      <c r="B19" s="49" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="26" t="s">
@@ -4122,7 +4122,7 @@
       </c>
     </row>
     <row r="20" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="40"/>
+      <c r="B20" s="50"/>
       <c r="C20" s="27" t="s">
         <v>23</v>
       </c>
@@ -4155,7 +4155,7 @@
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="40"/>
+      <c r="B21" s="50"/>
       <c r="C21" s="28" t="s">
         <v>26</v>
       </c>
@@ -4188,7 +4188,7 @@
       </c>
     </row>
     <row r="22" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="41"/>
+      <c r="B22" s="51"/>
       <c r="C22" s="27" t="s">
         <v>27</v>
       </c>
@@ -4221,7 +4221,7 @@
       </c>
     </row>
     <row r="23" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="39" t="s">
+      <c r="B23" s="49" t="s">
         <v>19</v>
       </c>
       <c r="C23" s="26" t="s">
@@ -4256,7 +4256,7 @@
       </c>
     </row>
     <row r="24" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="40"/>
+      <c r="B24" s="50"/>
       <c r="C24" s="27" t="s">
         <v>29</v>
       </c>
@@ -4289,7 +4289,7 @@
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B25" s="40"/>
+      <c r="B25" s="50"/>
       <c r="C25" s="26" t="s">
         <v>20</v>
       </c>
@@ -4322,7 +4322,7 @@
       </c>
     </row>
     <row r="26" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="41"/>
+      <c r="B26" s="51"/>
       <c r="C26" s="27" t="s">
         <v>21</v>
       </c>
@@ -4359,17 +4359,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="B7:B18"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="C16:C18"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E3:L3"/>
     <mergeCell ref="C4:D4"/>
@@ -4377,6 +4366,17 @@
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="B7:B18"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="61" orientation="landscape" verticalDpi="0" r:id="rId1"/>
@@ -4410,40 +4410,40 @@
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
     </row>
     <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E3" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="57"/>
-      <c r="L3" s="43"/>
+      <c r="E3" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="48"/>
     </row>
     <row r="4" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="F4" s="43"/>
-      <c r="G4" s="42" t="s">
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="48"/>
+      <c r="G4" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="43"/>
-      <c r="I4" s="42" t="s">
+      <c r="H4" s="48"/>
+      <c r="I4" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="43"/>
-      <c r="K4" s="42" t="s">
+      <c r="J4" s="48"/>
+      <c r="K4" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="L4" s="43"/>
+      <c r="L4" s="48"/>
     </row>
     <row r="5" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E5" s="37" t="s">
@@ -4478,28 +4478,28 @@
       <c r="D6" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="53" t="s">
+      <c r="E6" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="54"/>
-      <c r="G6" s="53" t="s">
+      <c r="F6" s="45"/>
+      <c r="G6" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="54"/>
-      <c r="I6" s="53" t="s">
+      <c r="H6" s="45"/>
+      <c r="I6" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="J6" s="54"/>
-      <c r="K6" s="53" t="s">
+      <c r="J6" s="45"/>
+      <c r="K6" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="L6" s="54"/>
+      <c r="L6" s="45"/>
     </row>
     <row r="7" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="44" t="s">
+      <c r="C7" s="52" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="12" t="s">
@@ -4531,8 +4531,8 @@
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="51"/>
-      <c r="C8" s="45"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="53"/>
       <c r="D8" s="13" t="s">
         <v>8</v>
       </c>
@@ -4562,8 +4562,8 @@
       </c>
     </row>
     <row r="9" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="51"/>
-      <c r="C9" s="46"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="54"/>
       <c r="D9" s="14" t="s">
         <v>9</v>
       </c>
@@ -4593,8 +4593,8 @@
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="51"/>
-      <c r="C10" s="44" t="s">
+      <c r="B10" s="59"/>
+      <c r="C10" s="52" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="12" t="s">
@@ -4626,8 +4626,8 @@
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="51"/>
-      <c r="C11" s="45"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="53"/>
       <c r="D11" s="13" t="s">
         <v>8</v>
       </c>
@@ -4657,8 +4657,8 @@
       </c>
     </row>
     <row r="12" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="51"/>
-      <c r="C12" s="46"/>
+      <c r="B12" s="59"/>
+      <c r="C12" s="54"/>
       <c r="D12" s="14" t="s">
         <v>9</v>
       </c>
@@ -4688,8 +4688,8 @@
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="51"/>
-      <c r="C13" s="44" t="s">
+      <c r="B13" s="59"/>
+      <c r="C13" s="52" t="s">
         <v>14</v>
       </c>
       <c r="D13" s="12" t="s">
@@ -4721,8 +4721,8 @@
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="51"/>
-      <c r="C14" s="45"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="53"/>
       <c r="D14" s="13" t="s">
         <v>8</v>
       </c>
@@ -4752,8 +4752,8 @@
       </c>
     </row>
     <row r="15" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="51"/>
-      <c r="C15" s="46"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="54"/>
       <c r="D15" s="14" t="s">
         <v>9</v>
       </c>
@@ -4783,8 +4783,8 @@
       </c>
     </row>
     <row r="16" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="51"/>
-      <c r="C16" s="47" t="s">
+      <c r="B16" s="59"/>
+      <c r="C16" s="55" t="s">
         <v>15</v>
       </c>
       <c r="D16" s="12" t="s">
@@ -4816,8 +4816,8 @@
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="51"/>
-      <c r="C17" s="48"/>
+      <c r="B17" s="59"/>
+      <c r="C17" s="56"/>
       <c r="D17" s="13" t="s">
         <v>8</v>
       </c>
@@ -4847,8 +4847,8 @@
       </c>
     </row>
     <row r="18" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="52"/>
-      <c r="C18" s="49"/>
+      <c r="B18" s="60"/>
+      <c r="C18" s="57"/>
       <c r="D18" s="14" t="s">
         <v>9</v>
       </c>
@@ -4878,7 +4878,7 @@
       </c>
     </row>
     <row r="19" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="39" t="s">
+      <c r="B19" s="49" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="26" t="s">
@@ -4913,7 +4913,7 @@
       </c>
     </row>
     <row r="20" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="40"/>
+      <c r="B20" s="50"/>
       <c r="C20" s="27" t="s">
         <v>23</v>
       </c>
@@ -4946,7 +4946,7 @@
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="40"/>
+      <c r="B21" s="50"/>
       <c r="C21" s="28" t="s">
         <v>26</v>
       </c>
@@ -4979,7 +4979,7 @@
       </c>
     </row>
     <row r="22" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="41"/>
+      <c r="B22" s="51"/>
       <c r="C22" s="27" t="s">
         <v>27</v>
       </c>
@@ -5012,7 +5012,7 @@
       </c>
     </row>
     <row r="23" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="39" t="s">
+      <c r="B23" s="49" t="s">
         <v>19</v>
       </c>
       <c r="C23" s="26" t="s">
@@ -5047,7 +5047,7 @@
       </c>
     </row>
     <row r="24" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="40"/>
+      <c r="B24" s="50"/>
       <c r="C24" s="27" t="s">
         <v>29</v>
       </c>
@@ -5080,7 +5080,7 @@
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B25" s="40"/>
+      <c r="B25" s="50"/>
       <c r="C25" s="26" t="s">
         <v>20</v>
       </c>
@@ -5113,7 +5113,7 @@
       </c>
     </row>
     <row r="26" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="41"/>
+      <c r="B26" s="51"/>
       <c r="C26" s="27" t="s">
         <v>21</v>
       </c>
@@ -5150,17 +5150,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="B7:B18"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="C16:C18"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E3:L3"/>
     <mergeCell ref="C4:D4"/>
@@ -5168,6 +5157,17 @@
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="B7:B18"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="61" orientation="landscape" verticalDpi="0" r:id="rId1"/>
@@ -5201,40 +5201,40 @@
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
     </row>
     <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E3" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="57"/>
-      <c r="L3" s="43"/>
+      <c r="E3" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="48"/>
     </row>
     <row r="4" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="F4" s="43"/>
-      <c r="G4" s="42" t="s">
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="48"/>
+      <c r="G4" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="43"/>
-      <c r="I4" s="42" t="s">
+      <c r="H4" s="48"/>
+      <c r="I4" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="43"/>
-      <c r="K4" s="42" t="s">
+      <c r="J4" s="48"/>
+      <c r="K4" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="L4" s="43"/>
+      <c r="L4" s="48"/>
     </row>
     <row r="5" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E5" s="37" t="s">
@@ -5269,28 +5269,28 @@
       <c r="D6" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="53" t="s">
+      <c r="E6" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="54"/>
-      <c r="G6" s="53" t="s">
+      <c r="F6" s="45"/>
+      <c r="G6" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="54"/>
-      <c r="I6" s="53" t="s">
+      <c r="H6" s="45"/>
+      <c r="I6" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="J6" s="54"/>
-      <c r="K6" s="53" t="s">
+      <c r="J6" s="45"/>
+      <c r="K6" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="L6" s="54"/>
+      <c r="L6" s="45"/>
     </row>
     <row r="7" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="44" t="s">
+      <c r="C7" s="52" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="12" t="s">
@@ -5322,8 +5322,8 @@
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="51"/>
-      <c r="C8" s="45"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="53"/>
       <c r="D8" s="13" t="s">
         <v>8</v>
       </c>
@@ -5353,8 +5353,8 @@
       </c>
     </row>
     <row r="9" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="51"/>
-      <c r="C9" s="46"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="54"/>
       <c r="D9" s="14" t="s">
         <v>9</v>
       </c>
@@ -5384,8 +5384,8 @@
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="51"/>
-      <c r="C10" s="44" t="s">
+      <c r="B10" s="59"/>
+      <c r="C10" s="52" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="12" t="s">
@@ -5417,8 +5417,8 @@
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="51"/>
-      <c r="C11" s="45"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="53"/>
       <c r="D11" s="13" t="s">
         <v>8</v>
       </c>
@@ -5448,8 +5448,8 @@
       </c>
     </row>
     <row r="12" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="51"/>
-      <c r="C12" s="46"/>
+      <c r="B12" s="59"/>
+      <c r="C12" s="54"/>
       <c r="D12" s="14" t="s">
         <v>9</v>
       </c>
@@ -5479,8 +5479,8 @@
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="51"/>
-      <c r="C13" s="44" t="s">
+      <c r="B13" s="59"/>
+      <c r="C13" s="52" t="s">
         <v>14</v>
       </c>
       <c r="D13" s="12" t="s">
@@ -5512,8 +5512,8 @@
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="51"/>
-      <c r="C14" s="45"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="53"/>
       <c r="D14" s="13" t="s">
         <v>8</v>
       </c>
@@ -5543,8 +5543,8 @@
       </c>
     </row>
     <row r="15" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="51"/>
-      <c r="C15" s="46"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="54"/>
       <c r="D15" s="14" t="s">
         <v>9</v>
       </c>
@@ -5574,8 +5574,8 @@
       </c>
     </row>
     <row r="16" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="51"/>
-      <c r="C16" s="47" t="s">
+      <c r="B16" s="59"/>
+      <c r="C16" s="55" t="s">
         <v>15</v>
       </c>
       <c r="D16" s="12" t="s">
@@ -5607,8 +5607,8 @@
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="51"/>
-      <c r="C17" s="48"/>
+      <c r="B17" s="59"/>
+      <c r="C17" s="56"/>
       <c r="D17" s="13" t="s">
         <v>8</v>
       </c>
@@ -5638,8 +5638,8 @@
       </c>
     </row>
     <row r="18" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="52"/>
-      <c r="C18" s="49"/>
+      <c r="B18" s="60"/>
+      <c r="C18" s="57"/>
       <c r="D18" s="14" t="s">
         <v>9</v>
       </c>
@@ -5669,7 +5669,7 @@
       </c>
     </row>
     <row r="19" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="39" t="s">
+      <c r="B19" s="49" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="26" t="s">
@@ -5704,7 +5704,7 @@
       </c>
     </row>
     <row r="20" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="40"/>
+      <c r="B20" s="50"/>
       <c r="C20" s="27" t="s">
         <v>23</v>
       </c>
@@ -5737,7 +5737,7 @@
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="40"/>
+      <c r="B21" s="50"/>
       <c r="C21" s="28" t="s">
         <v>26</v>
       </c>
@@ -5770,7 +5770,7 @@
       </c>
     </row>
     <row r="22" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="41"/>
+      <c r="B22" s="51"/>
       <c r="C22" s="27" t="s">
         <v>27</v>
       </c>
@@ -5803,7 +5803,7 @@
       </c>
     </row>
     <row r="23" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="39" t="s">
+      <c r="B23" s="49" t="s">
         <v>19</v>
       </c>
       <c r="C23" s="26" t="s">
@@ -5838,7 +5838,7 @@
       </c>
     </row>
     <row r="24" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="40"/>
+      <c r="B24" s="50"/>
       <c r="C24" s="27" t="s">
         <v>29</v>
       </c>
@@ -5871,7 +5871,7 @@
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B25" s="40"/>
+      <c r="B25" s="50"/>
       <c r="C25" s="26" t="s">
         <v>20</v>
       </c>
@@ -5904,7 +5904,7 @@
       </c>
     </row>
     <row r="26" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="41"/>
+      <c r="B26" s="51"/>
       <c r="C26" s="27" t="s">
         <v>21</v>
       </c>
@@ -5941,17 +5941,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="B7:B18"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="C16:C18"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E3:L3"/>
     <mergeCell ref="C4:D4"/>
@@ -5959,6 +5948,17 @@
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="B7:B18"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="61" orientation="landscape" verticalDpi="0" r:id="rId1"/>
@@ -5992,40 +5992,40 @@
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
     </row>
     <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E3" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="57"/>
-      <c r="L3" s="43"/>
+      <c r="E3" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="48"/>
     </row>
     <row r="4" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="F4" s="43"/>
-      <c r="G4" s="42" t="s">
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="48"/>
+      <c r="G4" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="43"/>
-      <c r="I4" s="42" t="s">
+      <c r="H4" s="48"/>
+      <c r="I4" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="43"/>
-      <c r="K4" s="42" t="s">
+      <c r="J4" s="48"/>
+      <c r="K4" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="L4" s="43"/>
+      <c r="L4" s="48"/>
     </row>
     <row r="5" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E5" s="37" t="s">
@@ -6060,28 +6060,28 @@
       <c r="D6" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="53" t="s">
+      <c r="E6" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="54"/>
-      <c r="G6" s="53" t="s">
+      <c r="F6" s="45"/>
+      <c r="G6" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="54"/>
-      <c r="I6" s="53" t="s">
+      <c r="H6" s="45"/>
+      <c r="I6" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="J6" s="54"/>
-      <c r="K6" s="53" t="s">
+      <c r="J6" s="45"/>
+      <c r="K6" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="L6" s="54"/>
+      <c r="L6" s="45"/>
     </row>
     <row r="7" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="44" t="s">
+      <c r="C7" s="52" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="12" t="s">
@@ -6113,8 +6113,8 @@
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="51"/>
-      <c r="C8" s="45"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="53"/>
       <c r="D8" s="13" t="s">
         <v>8</v>
       </c>
@@ -6144,8 +6144,8 @@
       </c>
     </row>
     <row r="9" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="51"/>
-      <c r="C9" s="46"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="54"/>
       <c r="D9" s="14" t="s">
         <v>9</v>
       </c>
@@ -6175,8 +6175,8 @@
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="51"/>
-      <c r="C10" s="44" t="s">
+      <c r="B10" s="59"/>
+      <c r="C10" s="52" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="12" t="s">
@@ -6208,8 +6208,8 @@
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="51"/>
-      <c r="C11" s="45"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="53"/>
       <c r="D11" s="13" t="s">
         <v>8</v>
       </c>
@@ -6239,8 +6239,8 @@
       </c>
     </row>
     <row r="12" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="51"/>
-      <c r="C12" s="46"/>
+      <c r="B12" s="59"/>
+      <c r="C12" s="54"/>
       <c r="D12" s="14" t="s">
         <v>9</v>
       </c>
@@ -6270,8 +6270,8 @@
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="51"/>
-      <c r="C13" s="44" t="s">
+      <c r="B13" s="59"/>
+      <c r="C13" s="52" t="s">
         <v>14</v>
       </c>
       <c r="D13" s="12" t="s">
@@ -6303,8 +6303,8 @@
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="51"/>
-      <c r="C14" s="45"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="53"/>
       <c r="D14" s="13" t="s">
         <v>8</v>
       </c>
@@ -6334,8 +6334,8 @@
       </c>
     </row>
     <row r="15" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="51"/>
-      <c r="C15" s="46"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="54"/>
       <c r="D15" s="14" t="s">
         <v>9</v>
       </c>
@@ -6365,8 +6365,8 @@
       </c>
     </row>
     <row r="16" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="51"/>
-      <c r="C16" s="47" t="s">
+      <c r="B16" s="59"/>
+      <c r="C16" s="55" t="s">
         <v>15</v>
       </c>
       <c r="D16" s="12" t="s">
@@ -6398,8 +6398,8 @@
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="51"/>
-      <c r="C17" s="48"/>
+      <c r="B17" s="59"/>
+      <c r="C17" s="56"/>
       <c r="D17" s="13" t="s">
         <v>8</v>
       </c>
@@ -6429,8 +6429,8 @@
       </c>
     </row>
     <row r="18" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="52"/>
-      <c r="C18" s="49"/>
+      <c r="B18" s="60"/>
+      <c r="C18" s="57"/>
       <c r="D18" s="14" t="s">
         <v>9</v>
       </c>
@@ -6460,7 +6460,7 @@
       </c>
     </row>
     <row r="19" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="39" t="s">
+      <c r="B19" s="49" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="26" t="s">
@@ -6495,7 +6495,7 @@
       </c>
     </row>
     <row r="20" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="40"/>
+      <c r="B20" s="50"/>
       <c r="C20" s="27" t="s">
         <v>23</v>
       </c>
@@ -6528,7 +6528,7 @@
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="40"/>
+      <c r="B21" s="50"/>
       <c r="C21" s="28" t="s">
         <v>26</v>
       </c>
@@ -6561,7 +6561,7 @@
       </c>
     </row>
     <row r="22" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="41"/>
+      <c r="B22" s="51"/>
       <c r="C22" s="27" t="s">
         <v>27</v>
       </c>
@@ -6594,7 +6594,7 @@
       </c>
     </row>
     <row r="23" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="39" t="s">
+      <c r="B23" s="49" t="s">
         <v>19</v>
       </c>
       <c r="C23" s="26" t="s">
@@ -6629,7 +6629,7 @@
       </c>
     </row>
     <row r="24" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="40"/>
+      <c r="B24" s="50"/>
       <c r="C24" s="27" t="s">
         <v>29</v>
       </c>
@@ -6662,7 +6662,7 @@
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B25" s="40"/>
+      <c r="B25" s="50"/>
       <c r="C25" s="26" t="s">
         <v>20</v>
       </c>
@@ -6695,7 +6695,7 @@
       </c>
     </row>
     <row r="26" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="41"/>
+      <c r="B26" s="51"/>
       <c r="C26" s="27" t="s">
         <v>21</v>
       </c>
@@ -6732,17 +6732,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="B7:B18"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="C16:C18"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E3:L3"/>
     <mergeCell ref="C4:D4"/>
@@ -6750,6 +6739,17 @@
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="B7:B18"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="61" orientation="landscape" verticalDpi="0" r:id="rId1"/>
@@ -6764,7 +6764,7 @@
   <dimension ref="B1:H57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+      <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6787,14 +6787,14 @@
       <c r="E2" s="11"/>
     </row>
     <row r="3" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E3" s="42"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="43"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="48"/>
     </row>
     <row r="4" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
       <c r="E4" s="23" t="s">
         <v>0</v>
       </c>
@@ -6804,7 +6804,7 @@
       <c r="G4" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="58" t="s">
+      <c r="H4" s="39" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6818,7 +6818,7 @@
       <c r="G5" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="H5" s="59" t="s">
+      <c r="H5" s="40" t="s">
         <v>40</v>
       </c>
     </row>
@@ -6838,15 +6838,15 @@
       <c r="G6" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="59" t="s">
+      <c r="H6" s="40" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="44" t="s">
+      <c r="C7" s="52" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="12" t="s">
@@ -6859,15 +6859,15 @@
         <v>211</v>
       </c>
       <c r="G7" s="15">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H7" s="12">
         <v>211</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="51"/>
-      <c r="C8" s="45"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="53"/>
       <c r="D8" s="13" t="s">
         <v>8</v>
       </c>
@@ -6885,8 +6885,8 @@
       </c>
     </row>
     <row r="9" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="51"/>
-      <c r="C9" s="46"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="54"/>
       <c r="D9" s="14" t="s">
         <v>9</v>
       </c>
@@ -6904,8 +6904,8 @@
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="51"/>
-      <c r="C10" s="44" t="s">
+      <c r="B10" s="59"/>
+      <c r="C10" s="52" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="12" t="s">
@@ -6925,8 +6925,8 @@
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="51"/>
-      <c r="C11" s="45"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="53"/>
       <c r="D11" s="13" t="s">
         <v>8</v>
       </c>
@@ -6944,8 +6944,8 @@
       </c>
     </row>
     <row r="12" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="51"/>
-      <c r="C12" s="46"/>
+      <c r="B12" s="59"/>
+      <c r="C12" s="54"/>
       <c r="D12" s="14" t="s">
         <v>9</v>
       </c>
@@ -6963,8 +6963,8 @@
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="51"/>
-      <c r="C13" s="44" t="s">
+      <c r="B13" s="59"/>
+      <c r="C13" s="52" t="s">
         <v>14</v>
       </c>
       <c r="D13" s="12" t="s">
@@ -6984,8 +6984,8 @@
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="51"/>
-      <c r="C14" s="45"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="53"/>
       <c r="D14" s="13" t="s">
         <v>8</v>
       </c>
@@ -7003,8 +7003,8 @@
       </c>
     </row>
     <row r="15" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="51"/>
-      <c r="C15" s="46"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="54"/>
       <c r="D15" s="14" t="s">
         <v>9</v>
       </c>
@@ -7022,8 +7022,8 @@
       </c>
     </row>
     <row r="16" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="51"/>
-      <c r="C16" s="47" t="s">
+      <c r="B16" s="59"/>
+      <c r="C16" s="55" t="s">
         <v>15</v>
       </c>
       <c r="D16" s="12" t="s">
@@ -7036,15 +7036,15 @@
         <v>100</v>
       </c>
       <c r="G16" s="15">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="H16" s="12">
         <v>100</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="51"/>
-      <c r="C17" s="48"/>
+      <c r="B17" s="59"/>
+      <c r="C17" s="56"/>
       <c r="D17" s="13" t="s">
         <v>8</v>
       </c>
@@ -7055,15 +7055,15 @@
         <v>100</v>
       </c>
       <c r="G17" s="17">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="H17" s="13">
         <v>100</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="52"/>
-      <c r="C18" s="49"/>
+      <c r="B18" s="60"/>
+      <c r="C18" s="57"/>
       <c r="D18" s="14" t="s">
         <v>9</v>
       </c>
@@ -7074,14 +7074,14 @@
         <v>100</v>
       </c>
       <c r="G18" s="19">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="H18" s="14">
         <v>100</v>
       </c>
     </row>
     <row r="19" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="39" t="s">
+      <c r="B19" s="49" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="26" t="s">
@@ -7099,12 +7099,12 @@
       <c r="G19" s="33">
         <v>46</v>
       </c>
-      <c r="H19" s="60">
+      <c r="H19" s="41">
         <v>46</v>
       </c>
     </row>
     <row r="20" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="40"/>
+      <c r="B20" s="50"/>
       <c r="C20" s="27" t="s">
         <v>23</v>
       </c>
@@ -7120,12 +7120,12 @@
       <c r="G20" s="31">
         <v>98</v>
       </c>
-      <c r="H20" s="61">
+      <c r="H20" s="42">
         <v>98</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="40"/>
+      <c r="B21" s="50"/>
       <c r="C21" s="28" t="s">
         <v>26</v>
       </c>
@@ -7141,12 +7141,12 @@
       <c r="G21" s="33">
         <v>2031</v>
       </c>
-      <c r="H21" s="60">
+      <c r="H21" s="41">
         <v>2031</v>
       </c>
     </row>
     <row r="22" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="41"/>
+      <c r="B22" s="51"/>
       <c r="C22" s="27" t="s">
         <v>27</v>
       </c>
@@ -7162,12 +7162,12 @@
       <c r="G22" s="31">
         <v>2021</v>
       </c>
-      <c r="H22" s="61">
+      <c r="H22" s="42">
         <v>2021</v>
       </c>
     </row>
     <row r="23" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="39" t="s">
+      <c r="B23" s="49" t="s">
         <v>19</v>
       </c>
       <c r="C23" s="26" t="s">
@@ -7185,12 +7185,12 @@
       <c r="G23" s="33">
         <v>2043</v>
       </c>
-      <c r="H23" s="60">
+      <c r="H23" s="41">
         <v>2044</v>
       </c>
     </row>
     <row r="24" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="40"/>
+      <c r="B24" s="50"/>
       <c r="C24" s="27" t="s">
         <v>29</v>
       </c>
@@ -7204,14 +7204,14 @@
         <v>2025</v>
       </c>
       <c r="G24" s="31">
-        <v>2024</v>
-      </c>
-      <c r="H24" s="61">
         <v>2025</v>
       </c>
+      <c r="H24" s="42">
+        <v>2025</v>
+      </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="40"/>
+      <c r="B25" s="50"/>
       <c r="C25" s="26" t="s">
         <v>20</v>
       </c>
@@ -7227,12 +7227,12 @@
       <c r="G25" s="33">
         <v>8</v>
       </c>
-      <c r="H25" s="60">
+      <c r="H25" s="41">
         <v>10</v>
       </c>
     </row>
     <row r="26" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="41"/>
+      <c r="B26" s="51"/>
       <c r="C26" s="27" t="s">
         <v>21</v>
       </c>
@@ -7248,7 +7248,7 @@
       <c r="G26" s="31">
         <v>0</v>
       </c>
-      <c r="H26" s="61">
+      <c r="H26" s="42">
         <v>0</v>
       </c>
     </row>
@@ -7262,6 +7262,8 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="C4:D4"/>
     <mergeCell ref="B19:B22"/>
     <mergeCell ref="B23:B26"/>
     <mergeCell ref="B7:B18"/>
@@ -7269,8 +7271,6 @@
     <mergeCell ref="C10:C12"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="C16:C18"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="C4:D4"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="61" orientation="landscape" verticalDpi="0" r:id="rId1"/>

</xml_diff>